<commit_message>
Update de Operations.js y update del excel
</commit_message>
<xml_diff>
--- a/No Code/Calculo Mermelada.xlsx
+++ b/No Code/Calculo Mermelada.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\No Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D5F742-A35A-4610-B3F2-D2AF5DABC120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C8C411-2AB4-424C-A4F2-D78D84A29BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>PROCESO 1 LAVADO Y PELADO</t>
   </si>
@@ -102,13 +102,32 @@
   </si>
   <si>
     <t>PROCESO 3 MACHACADO</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Manzana</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,7 +136,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +158,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,10 +192,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,15 +225,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C596F734-F118-46F5-8754-D9959929CA75}">
-  <dimension ref="A2:J22"/>
+  <dimension ref="A2:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,36 +569,45 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="12"/>
+      <c r="I2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M2" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -576,30 +615,39 @@
         <v>436</v>
       </c>
       <c r="C3" s="7">
-        <f>H3</f>
-        <v>436</v>
+        <f>I3</f>
+        <v>1</v>
       </c>
       <c r="D3" s="7">
         <f>D21*(436/325)</f>
-        <v>436</v>
+        <v>1.3415384615384616</v>
       </c>
       <c r="E3" s="7">
         <f>(E20*436)/F20</f>
-        <v>436.00075899638239</v>
-      </c>
-      <c r="H3" s="3">
-        <v>436</v>
-      </c>
-      <c r="I3" s="7">
+        <v>2.4482046100083177</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
         <f>C20</f>
-        <v>178.08968997837059</v>
-      </c>
-      <c r="J3" s="7">
+        <v>0.40252293577981652</v>
+      </c>
+      <c r="K3" s="7">
         <f>C21</f>
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.74541284403669728</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -607,19 +655,40 @@
         <v>44</v>
       </c>
       <c r="C4" s="7">
-        <f>C3*(((44*100)/436)/100)</f>
-        <v>44</v>
+        <f>C3*(((47*100)/436)/100)</f>
+        <v>0.10779816513761467</v>
       </c>
       <c r="D4" s="7">
         <f>D3*(((44*100)/436)/100)</f>
-        <v>44</v>
+        <v>0.13538461538461541</v>
       </c>
       <c r="E4" s="7">
         <f>E3*(((44*100)/436)/100)</f>
-        <v>44.000076595965197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.24706652027606876</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="14">
+        <f>I3*N2</f>
+        <v>50</v>
+      </c>
+      <c r="J4" s="14">
+        <f>J3*N2</f>
+        <v>20.126146788990827</v>
+      </c>
+      <c r="K4" s="15">
+        <f>K3*N4</f>
+        <v>52.178899082568812</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -635,111 +704,110 @@
       <c r="E5" s="7">
         <v>331</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C6" s="7">
         <f>C3-C4</f>
-        <v>392</v>
+        <v>0.89220183486238536</v>
       </c>
       <c r="D6" s="7">
         <f>D3-D4</f>
-        <v>392</v>
+        <v>1.2061538461538461</v>
       </c>
       <c r="E6" s="7">
         <f>E3-E4</f>
-        <v>392.00068240041719</v>
-      </c>
-      <c r="H6" s="8">
-        <v>325</v>
-      </c>
-      <c r="I6" s="9">
-        <f>H6*(436/325)</f>
-        <v>436</v>
-      </c>
-      <c r="J6" s="9">
-        <f>D20</f>
-        <v>178.08968997837059</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.201138089732249</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="11" t="s">
+      <c r="H8" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="8">
         <v>1</v>
       </c>
-      <c r="J8" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J8" s="9">
+        <f>I8*(436/325)</f>
+        <v>1.3415384615384616</v>
+      </c>
+      <c r="K8" s="9">
+        <f>D20</f>
+        <v>0.54796827685652494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3">
         <f>B6</f>
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C9" s="7">
         <f>C6</f>
-        <v>392</v>
+        <v>0.89220183486238536</v>
       </c>
       <c r="D9" s="7">
         <f>D6</f>
-        <v>392</v>
+        <v>1.2061538461538461</v>
       </c>
       <c r="E9" s="7">
         <f>E6</f>
-        <v>392.00068240041719</v>
-      </c>
-      <c r="H9" s="8">
-        <v>178.09</v>
-      </c>
-      <c r="I9" s="9">
-        <f>E3</f>
-        <v>436.00075899638239</v>
-      </c>
-      <c r="J9" s="9">
-        <f>E21</f>
-        <v>325.00056576565203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.201138089732249</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="15">
+        <f>I8*N4</f>
+        <v>70</v>
+      </c>
+      <c r="J9" s="14">
+        <f>J8*N2</f>
+        <v>67.07692307692308</v>
+      </c>
+      <c r="K9" s="14">
+        <f>K8*N3</f>
+        <v>10.959365537130498</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -747,19 +815,19 @@
         <v>22</v>
       </c>
       <c r="C10" s="7">
-        <f>C9*(((22*100)/399)/100)</f>
-        <v>21.614035087719301</v>
+        <f>C9*(((24*100)/389)/100)</f>
+        <v>5.5045871559633031E-2</v>
       </c>
       <c r="D10" s="7">
         <f>D9*(((22*100)/399)/100)</f>
-        <v>21.614035087719301</v>
+        <v>6.6504723346828609E-2</v>
       </c>
       <c r="E10" s="7">
         <f>E9*(((22*100)/399)/100)</f>
-        <v>21.614072713807467</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.12136600996017415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -768,40 +836,64 @@
       </c>
       <c r="C11" s="7">
         <f>C9-C10</f>
-        <v>370.38596491228071</v>
+        <v>0.83715596330275233</v>
       </c>
       <c r="D11" s="7">
         <f>D9-D10</f>
-        <v>370.38596491228071</v>
+        <v>1.1396491228070176</v>
       </c>
       <c r="E11" s="7">
         <f>E9-E10</f>
-        <v>370.38660968660975</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0797720797720749</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="9">
+        <f>E3</f>
+        <v>2.4482046100083177</v>
+      </c>
+      <c r="K13" s="9">
+        <f>E21</f>
+        <v>1.8249231611300534</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -811,18 +903,33 @@
       </c>
       <c r="C14" s="7">
         <f>C11</f>
-        <v>370.38596491228071</v>
+        <v>0.83715596330275233</v>
       </c>
       <c r="D14" s="7">
         <f>D11</f>
-        <v>370.38596491228071</v>
+        <v>1.1396491228070176</v>
       </c>
       <c r="E14" s="7">
         <f>E11</f>
-        <v>370.38660968660975</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.0797720797720749</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="14">
+        <f>I13*N3</f>
+        <v>20</v>
+      </c>
+      <c r="J14" s="14">
+        <f>J13*N2</f>
+        <v>122.41023050041588</v>
+      </c>
+      <c r="K14" s="15">
+        <f>K13*N4</f>
+        <v>127.74462127910374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -831,18 +938,18 @@
       </c>
       <c r="C15" s="7">
         <f>C14*(((14*100)/365)/100)</f>
-        <v>14.206584955539533</v>
+        <v>3.2110091743119261E-2</v>
       </c>
       <c r="D15" s="7">
         <f>D14*(((14*100)/365)/100)</f>
-        <v>14.206584955539533</v>
+        <v>4.3712569093967792E-2</v>
       </c>
       <c r="E15" s="7">
         <f>E14*(((14*100)/365)/100)</f>
-        <v>14.206609686609687</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7.9772079772079577E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -851,41 +958,40 @@
       </c>
       <c r="C16" s="7">
         <f>C14-C15</f>
-        <v>356.17937995674117</v>
+        <v>0.80504587155963303</v>
       </c>
       <c r="D16" s="7">
         <f>D14-D15</f>
-        <v>356.17937995674117</v>
+        <v>1.0959365537130499</v>
       </c>
       <c r="E16" s="7">
         <f>E14-E15</f>
-        <v>356.18000000000006</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.9999999999999953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
@@ -895,18 +1001,18 @@
       </c>
       <c r="C19" s="7">
         <f>C16</f>
-        <v>356.17937995674117</v>
+        <v>0.80504587155963303</v>
       </c>
       <c r="D19" s="7">
         <f>D16</f>
-        <v>356.17937995674117</v>
+        <v>1.0959365537130499</v>
       </c>
       <c r="E19" s="7">
         <f>E16</f>
-        <v>356.18000000000006</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.9999999999999953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -916,21 +1022,21 @@
       </c>
       <c r="C20" s="7">
         <f>C19/2</f>
-        <v>178.08968997837059</v>
+        <v>0.40252293577981652</v>
       </c>
       <c r="D20" s="7">
         <f>D19/2</f>
-        <v>178.08968997837059</v>
+        <v>0.54796827685652494</v>
       </c>
       <c r="E20" s="7">
-        <f>H9</f>
-        <v>178.09</v>
+        <f>I13</f>
+        <v>1</v>
       </c>
       <c r="F20">
-        <v>178.08968997837059</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>178.08968997837101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -939,18 +1045,18 @@
       </c>
       <c r="C21" s="7">
         <f>C3*(325/436)</f>
-        <v>325</v>
+        <v>0.74541284403669728</v>
       </c>
       <c r="D21" s="7">
-        <f>H6</f>
-        <v>325</v>
+        <f>I8</f>
+        <v>1</v>
       </c>
       <c r="E21" s="7">
         <f>E3*(325/436)</f>
-        <v>325.00056576565203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.8249231611300534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -959,15 +1065,15 @@
       </c>
       <c r="C22" s="7">
         <f>(C19+C20)-C21</f>
-        <v>209.2690699351117</v>
+        <v>0.46215596330275222</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" ref="D22:E22" si="0">(D19+D20)-D21</f>
-        <v>209.2690699351117</v>
+        <v>0.64390483056957493</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" si="0"/>
-        <v>209.26943423434807</v>
+        <f>(E19+E20)-E21</f>
+        <v>1.1750768388699422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update en Operations.js para regresar con precios
</commit_message>
<xml_diff>
--- a/No Code/Calculo Mermelada.xlsx
+++ b/No Code/Calculo Mermelada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\No Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C8C411-2AB4-424C-A4F2-D78D84A29BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614EF8B0-DE79-410D-9940-6E980FE01D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,29 +616,29 @@
       </c>
       <c r="C3" s="7">
         <f>I3</f>
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="D3" s="7">
         <f>D21*(436/325)</f>
-        <v>1.3415384615384616</v>
+        <v>670.76923076923083</v>
       </c>
       <c r="E3" s="7">
         <f>(E20*436)/F20</f>
-        <v>2.4482046100083177</v>
+        <v>244.82046100083176</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="3">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="J3" s="7">
         <f>C20</f>
-        <v>0.40252293577981652</v>
+        <v>201.26146788990826</v>
       </c>
       <c r="K3" s="7">
         <f>C21</f>
-        <v>0.74541284403669728</v>
+        <v>372.70642201834863</v>
       </c>
       <c r="M3" s="10" t="s">
         <v>12</v>
@@ -656,30 +656,30 @@
       </c>
       <c r="C4" s="7">
         <f>C3*(((47*100)/436)/100)</f>
-        <v>0.10779816513761467</v>
+        <v>53.899082568807337</v>
       </c>
       <c r="D4" s="7">
         <f>D3*(((44*100)/436)/100)</f>
-        <v>0.13538461538461541</v>
+        <v>67.692307692307708</v>
       </c>
       <c r="E4" s="7">
         <f>E3*(((44*100)/436)/100)</f>
-        <v>0.24706652027606876</v>
+        <v>24.706652027606875</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="14">
         <f>I3*N2</f>
-        <v>50</v>
+        <v>25000</v>
       </c>
       <c r="J4" s="14">
         <f>J3*N2</f>
-        <v>20.126146788990827</v>
+        <v>10063.073394495414</v>
       </c>
       <c r="K4" s="15">
         <f>K3*N4</f>
-        <v>52.178899082568812</v>
+        <v>26089.449541284404</v>
       </c>
       <c r="M4" s="10" t="s">
         <v>13</v>
@@ -714,15 +714,15 @@
       </c>
       <c r="C6" s="7">
         <f>C3-C4</f>
-        <v>0.89220183486238536</v>
+        <v>446.10091743119267</v>
       </c>
       <c r="D6" s="7">
         <f>D3-D4</f>
-        <v>1.2061538461538461</v>
+        <v>603.07692307692309</v>
       </c>
       <c r="E6" s="7">
         <f>E3-E4</f>
-        <v>2.201138089732249</v>
+        <v>220.11380897322488</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -760,15 +760,15 @@
         <v>23</v>
       </c>
       <c r="I8" s="8">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="J8" s="9">
         <f>I8*(436/325)</f>
-        <v>1.3415384615384616</v>
+        <v>670.76923076923083</v>
       </c>
       <c r="K8" s="9">
         <f>D20</f>
-        <v>0.54796827685652494</v>
+        <v>273.98413842826244</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -781,30 +781,30 @@
       </c>
       <c r="C9" s="7">
         <f>C6</f>
-        <v>0.89220183486238536</v>
+        <v>446.10091743119267</v>
       </c>
       <c r="D9" s="7">
         <f>D6</f>
-        <v>1.2061538461538461</v>
+        <v>603.07692307692309</v>
       </c>
       <c r="E9" s="7">
         <f>E6</f>
-        <v>2.201138089732249</v>
+        <v>220.11380897322488</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I9" s="15">
         <f>I8*N4</f>
-        <v>70</v>
+        <v>35000</v>
       </c>
       <c r="J9" s="14">
         <f>J8*N2</f>
-        <v>67.07692307692308</v>
+        <v>33538.461538461539</v>
       </c>
       <c r="K9" s="14">
         <f>K8*N3</f>
-        <v>10.959365537130498</v>
+        <v>5479.6827685652488</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -816,15 +816,15 @@
       </c>
       <c r="C10" s="7">
         <f>C9*(((24*100)/389)/100)</f>
-        <v>5.5045871559633031E-2</v>
+        <v>27.522935779816514</v>
       </c>
       <c r="D10" s="7">
         <f>D9*(((22*100)/399)/100)</f>
-        <v>6.6504723346828609E-2</v>
+        <v>33.252361673414306</v>
       </c>
       <c r="E10" s="7">
         <f>E9*(((22*100)/399)/100)</f>
-        <v>0.12136600996017415</v>
+        <v>12.136600996017412</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,15 +836,15 @@
       </c>
       <c r="C11" s="7">
         <f>C9-C10</f>
-        <v>0.83715596330275233</v>
+        <v>418.57798165137615</v>
       </c>
       <c r="D11" s="7">
         <f>D9-D10</f>
-        <v>1.1396491228070176</v>
+        <v>569.82456140350882</v>
       </c>
       <c r="E11" s="7">
         <f>E9-E10</f>
-        <v>2.0797720797720749</v>
+        <v>207.97720797720746</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -882,15 +882,15 @@
         <v>23</v>
       </c>
       <c r="I13" s="8">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="J13" s="9">
         <f>E3</f>
-        <v>2.4482046100083177</v>
+        <v>244.82046100083176</v>
       </c>
       <c r="K13" s="9">
         <f>E21</f>
-        <v>1.8249231611300534</v>
+        <v>182.49231611300533</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -903,30 +903,30 @@
       </c>
       <c r="C14" s="7">
         <f>C11</f>
-        <v>0.83715596330275233</v>
+        <v>418.57798165137615</v>
       </c>
       <c r="D14" s="7">
         <f>D11</f>
-        <v>1.1396491228070176</v>
+        <v>569.82456140350882</v>
       </c>
       <c r="E14" s="7">
         <f>E11</f>
-        <v>2.0797720797720749</v>
+        <v>207.97720797720746</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="14">
         <f>I13*N3</f>
-        <v>20</v>
+        <v>2000</v>
       </c>
       <c r="J14" s="14">
         <f>J13*N2</f>
-        <v>122.41023050041588</v>
+        <v>12241.023050041587</v>
       </c>
       <c r="K14" s="15">
         <f>K13*N4</f>
-        <v>127.74462127910374</v>
+        <v>12774.462127910374</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -938,15 +938,15 @@
       </c>
       <c r="C15" s="7">
         <f>C14*(((14*100)/365)/100)</f>
-        <v>3.2110091743119261E-2</v>
+        <v>16.055045871559631</v>
       </c>
       <c r="D15" s="7">
         <f>D14*(((14*100)/365)/100)</f>
-        <v>4.3712569093967792E-2</v>
+        <v>21.856284546983897</v>
       </c>
       <c r="E15" s="7">
         <f>E14*(((14*100)/365)/100)</f>
-        <v>7.9772079772079577E-2</v>
+        <v>7.9772079772079563</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -958,15 +958,15 @@
       </c>
       <c r="C16" s="7">
         <f>C14-C15</f>
-        <v>0.80504587155963303</v>
+        <v>402.52293577981652</v>
       </c>
       <c r="D16" s="7">
         <f>D14-D15</f>
-        <v>1.0959365537130499</v>
+        <v>547.96827685652488</v>
       </c>
       <c r="E16" s="7">
         <f>E14-E15</f>
-        <v>1.9999999999999953</v>
+        <v>199.99999999999949</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,15 +1001,15 @@
       </c>
       <c r="C19" s="7">
         <f>C16</f>
-        <v>0.80504587155963303</v>
+        <v>402.52293577981652</v>
       </c>
       <c r="D19" s="7">
         <f>D16</f>
-        <v>1.0959365537130499</v>
+        <v>547.96827685652488</v>
       </c>
       <c r="E19" s="7">
         <f>E16</f>
-        <v>1.9999999999999953</v>
+        <v>199.99999999999949</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,15 +1022,15 @@
       </c>
       <c r="C20" s="7">
         <f>C19/2</f>
-        <v>0.40252293577981652</v>
+        <v>201.26146788990826</v>
       </c>
       <c r="D20" s="7">
         <f>D19/2</f>
-        <v>0.54796827685652494</v>
+        <v>273.98413842826244</v>
       </c>
       <c r="E20" s="7">
         <f>I13</f>
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="F20">
         <v>178.08968997837101</v>
@@ -1045,15 +1045,15 @@
       </c>
       <c r="C21" s="7">
         <f>C3*(325/436)</f>
-        <v>0.74541284403669728</v>
+        <v>372.70642201834863</v>
       </c>
       <c r="D21" s="7">
         <f>I8</f>
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E21" s="7">
         <f>E3*(325/436)</f>
-        <v>1.8249231611300534</v>
+        <v>182.49231611300533</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1065,15 +1065,15 @@
       </c>
       <c r="C22" s="7">
         <f>(C19+C20)-C21</f>
-        <v>0.46215596330275222</v>
+        <v>231.07798165137609</v>
       </c>
       <c r="D22" s="7">
-        <f t="shared" ref="D22:E22" si="0">(D19+D20)-D21</f>
-        <v>0.64390483056957493</v>
+        <f t="shared" ref="D22" si="0">(D19+D20)-D21</f>
+        <v>321.95241528478732</v>
       </c>
       <c r="E22" s="7">
         <f>(E19+E20)-E21</f>
-        <v>1.1750768388699422</v>
+        <v>117.50768388699416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update de Operation.js agregando utilidades el return y update del excel
</commit_message>
<xml_diff>
--- a/No Code/Calculo Mermelada.xlsx
+++ b/No Code/Calculo Mermelada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\No Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614EF8B0-DE79-410D-9940-6E980FE01D5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D579DC-01AA-41BD-871A-6D9BBA53328B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
   <si>
     <t>PROCESO 1 LAVADO Y PELADO</t>
   </si>
@@ -111,14 +111,34 @@
   </si>
   <si>
     <t>Manzana</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>Invertido</t>
+  </si>
+  <si>
+    <t>Ganado</t>
+  </si>
+  <si>
+    <t>Utilidad</t>
+  </si>
+  <si>
+    <t>Egresos</t>
+  </si>
+  <si>
+    <t>Ingresos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="172" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -136,7 +156,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -196,7 +222,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,9 +258,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -558,20 +590,22 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -600,11 +634,9 @@
       <c r="K2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="13">
-        <v>50</v>
+      <c r="M2" s="12"/>
+      <c r="N2" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -615,16 +647,15 @@
         <v>436</v>
       </c>
       <c r="C3" s="7">
-        <f>I3</f>
-        <v>500</v>
+        <v>436</v>
       </c>
       <c r="D3" s="7">
         <f>D21*(436/325)</f>
-        <v>670.76923076923083</v>
+        <v>436</v>
       </c>
       <c r="E3" s="7">
-        <f>(E20*436)/F20</f>
-        <v>244.82046100083176</v>
+        <f>(E20*436)/175.5</f>
+        <v>436</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>23</v>
@@ -634,17 +665,18 @@
       </c>
       <c r="J3" s="7">
         <f>C20</f>
-        <v>201.26146788990826</v>
-      </c>
-      <c r="K3" s="7">
+        <v>175.5</v>
+      </c>
+      <c r="K3" s="19">
         <f>C21</f>
-        <v>372.70642201834863</v>
+        <v>325</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="13">
-        <v>20</v>
+        <v>29</v>
+      </c>
+      <c r="N3" s="16">
+        <f>J4+I4</f>
+        <v>28510</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -656,36 +688,38 @@
       </c>
       <c r="C4" s="7">
         <f>C3*(((47*100)/436)/100)</f>
-        <v>53.899082568807337</v>
+        <v>47</v>
       </c>
       <c r="D4" s="7">
-        <f>D3*(((44*100)/436)/100)</f>
-        <v>67.692307692307708</v>
+        <f>D3*(((47*100)/436)/100)</f>
+        <v>47</v>
       </c>
       <c r="E4" s="7">
-        <f>E3*(((44*100)/436)/100)</f>
-        <v>24.706652027606875</v>
+        <f>E3*(((47*100)/436)/100)</f>
+        <v>47</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="14">
-        <f>I3*N2</f>
+      <c r="I4" s="16">
+        <f>I3*I17</f>
         <v>25000</v>
       </c>
-      <c r="J4" s="14">
-        <f>J3*N2</f>
-        <v>10063.073394495414</v>
-      </c>
-      <c r="K4" s="15">
-        <f>K3*N4</f>
-        <v>26089.449541284404</v>
-      </c>
+      <c r="J4" s="16">
+        <f>I18*J3</f>
+        <v>3510</v>
+      </c>
+      <c r="K4" s="17">
+        <f>K3*I19</f>
+        <v>32500</v>
+      </c>
+      <c r="L4" s="13"/>
       <c r="M4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="13">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="N4" s="17">
+        <f>K4</f>
+        <v>32500</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -704,6 +738,13 @@
       <c r="E5" s="7">
         <v>331</v>
       </c>
+      <c r="M5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="15">
+        <f>N4-N3</f>
+        <v>3990</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
@@ -714,15 +755,15 @@
       </c>
       <c r="C6" s="7">
         <f>C3-C4</f>
-        <v>446.10091743119267</v>
+        <v>389</v>
       </c>
       <c r="D6" s="7">
         <f>D3-D4</f>
-        <v>603.07692307692309</v>
+        <v>389</v>
       </c>
       <c r="E6" s="7">
         <f>E3-E4</f>
-        <v>220.11380897322488</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -739,6 +780,10 @@
       <c r="K7" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="M7" s="12"/>
+      <c r="N7" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -760,15 +805,22 @@
         <v>23</v>
       </c>
       <c r="I8" s="8">
-        <v>500</v>
+        <v>325</v>
       </c>
       <c r="J8" s="9">
         <f>I8*(436/325)</f>
-        <v>670.76923076923083</v>
+        <v>436</v>
       </c>
       <c r="K8" s="9">
         <f>D20</f>
-        <v>273.98413842826244</v>
+        <v>175.5</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N8" s="16">
+        <f>J9+K9</f>
+        <v>25310</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -781,30 +833,38 @@
       </c>
       <c r="C9" s="7">
         <f>C6</f>
-        <v>446.10091743119267</v>
+        <v>389</v>
       </c>
       <c r="D9" s="7">
         <f>D6</f>
-        <v>603.07692307692309</v>
+        <v>389</v>
       </c>
       <c r="E9" s="7">
         <f>E6</f>
-        <v>220.11380897322488</v>
+        <v>389</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I9" s="15">
-        <f>I8*N4</f>
-        <v>35000</v>
-      </c>
-      <c r="J9" s="14">
-        <f>J8*N2</f>
-        <v>33538.461538461539</v>
-      </c>
-      <c r="K9" s="14">
-        <f>K8*N3</f>
-        <v>5479.6827685652488</v>
+      <c r="I9" s="17">
+        <f>I8*I19</f>
+        <v>32500</v>
+      </c>
+      <c r="J9" s="16">
+        <f>J8*I17</f>
+        <v>21800</v>
+      </c>
+      <c r="K9" s="16">
+        <f>K8*I18</f>
+        <v>3510</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="17">
+        <f>I9</f>
+        <v>32500</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -816,15 +876,22 @@
       </c>
       <c r="C10" s="7">
         <f>C9*(((24*100)/389)/100)</f>
-        <v>27.522935779816514</v>
+        <v>24</v>
       </c>
       <c r="D10" s="7">
-        <f>D9*(((22*100)/399)/100)</f>
-        <v>33.252361673414306</v>
+        <f>D9*(((24*100)/389)/100)</f>
+        <v>24</v>
       </c>
       <c r="E10" s="7">
-        <f>E9*(((22*100)/399)/100)</f>
-        <v>12.136600996017412</v>
+        <f>E9*(((24*100)/389)/100)</f>
+        <v>24</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="15">
+        <f>N9-N8</f>
+        <v>7190</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -836,15 +903,15 @@
       </c>
       <c r="C11" s="7">
         <f>C9-C10</f>
-        <v>418.57798165137615</v>
+        <v>365</v>
       </c>
       <c r="D11" s="7">
         <f>D9-D10</f>
-        <v>569.82456140350882</v>
+        <v>365</v>
       </c>
       <c r="E11" s="7">
         <f>E9-E10</f>
-        <v>207.97720797720746</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -861,6 +928,10 @@
       <c r="K12" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="M12" s="12"/>
+      <c r="N12" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -882,15 +953,22 @@
         <v>23</v>
       </c>
       <c r="I13" s="8">
-        <v>100</v>
+        <v>175.5</v>
       </c>
       <c r="J13" s="9">
         <f>E3</f>
-        <v>244.82046100083176</v>
+        <v>436</v>
       </c>
       <c r="K13" s="9">
         <f>E21</f>
-        <v>182.49231611300533</v>
+        <v>325</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="16">
+        <f>J14+I14</f>
+        <v>25310</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -903,30 +981,38 @@
       </c>
       <c r="C14" s="7">
         <f>C11</f>
-        <v>418.57798165137615</v>
+        <v>365</v>
       </c>
       <c r="D14" s="7">
         <f>D11</f>
-        <v>569.82456140350882</v>
+        <v>365</v>
       </c>
       <c r="E14" s="7">
         <f>E11</f>
-        <v>207.97720797720746</v>
+        <v>365</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="14">
-        <f>I13*N3</f>
-        <v>2000</v>
-      </c>
-      <c r="J14" s="14">
-        <f>J13*N2</f>
-        <v>12241.023050041587</v>
-      </c>
-      <c r="K14" s="15">
-        <f>K13*N4</f>
-        <v>12774.462127910374</v>
+      <c r="I14" s="16">
+        <f>I13*I18</f>
+        <v>3510</v>
+      </c>
+      <c r="J14" s="16">
+        <f>J13*I17</f>
+        <v>21800</v>
+      </c>
+      <c r="K14" s="17">
+        <f>K13*I19</f>
+        <v>32500</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="17">
+        <f>K14</f>
+        <v>32500</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -938,15 +1024,22 @@
       </c>
       <c r="C15" s="7">
         <f>C14*(((14*100)/365)/100)</f>
-        <v>16.055045871559631</v>
+        <v>13.999999999999998</v>
       </c>
       <c r="D15" s="7">
         <f>D14*(((14*100)/365)/100)</f>
-        <v>21.856284546983897</v>
+        <v>13.999999999999998</v>
       </c>
       <c r="E15" s="7">
         <f>E14*(((14*100)/365)/100)</f>
-        <v>7.9772079772079563</v>
+        <v>13.999999999999998</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="15">
+        <f>N14-N13</f>
+        <v>7190</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -958,23 +1051,32 @@
       </c>
       <c r="C16" s="7">
         <f>C14-C15</f>
-        <v>402.52293577981652</v>
+        <v>351</v>
       </c>
       <c r="D16" s="7">
         <f>D14-D15</f>
-        <v>547.96827685652488</v>
+        <v>351</v>
       </c>
       <c r="E16" s="7">
         <f>E14-E15</f>
-        <v>199.99999999999949</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H17" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
@@ -990,8 +1092,14 @@
       <c r="E18" s="10" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1001,18 +1109,24 @@
       </c>
       <c r="C19" s="7">
         <f>C16</f>
-        <v>402.52293577981652</v>
+        <v>351</v>
       </c>
       <c r="D19" s="7">
         <f>D16</f>
-        <v>547.96827685652488</v>
+        <v>351</v>
       </c>
       <c r="E19" s="7">
         <f>E16</f>
-        <v>199.99999999999949</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1022,21 +1136,18 @@
       </c>
       <c r="C20" s="7">
         <f>C19/2</f>
-        <v>201.26146788990826</v>
+        <v>175.5</v>
       </c>
       <c r="D20" s="7">
         <f>D19/2</f>
-        <v>273.98413842826244</v>
+        <v>175.5</v>
       </c>
       <c r="E20" s="7">
         <f>I13</f>
-        <v>100</v>
-      </c>
-      <c r="F20">
-        <v>178.08968997837101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>175.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -1045,18 +1156,18 @@
       </c>
       <c r="C21" s="7">
         <f>C3*(325/436)</f>
-        <v>372.70642201834863</v>
+        <v>325</v>
       </c>
       <c r="D21" s="7">
         <f>I8</f>
-        <v>500</v>
+        <v>325</v>
       </c>
       <c r="E21" s="7">
         <f>E3*(325/436)</f>
-        <v>182.49231611300533</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
@@ -1065,15 +1176,15 @@
       </c>
       <c r="C22" s="7">
         <f>(C19+C20)-C21</f>
-        <v>231.07798165137609</v>
+        <v>201.5</v>
       </c>
       <c r="D22" s="7">
         <f t="shared" ref="D22" si="0">(D19+D20)-D21</f>
-        <v>321.95241528478732</v>
+        <v>201.5</v>
       </c>
       <c r="E22" s="7">
         <f>(E19+E20)-E21</f>
-        <v>117.50768388699416</v>
+        <v>201.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
backend y frotend funcionando correctamente y pasando los reslutados correctos
</commit_message>
<xml_diff>
--- a/No Code/Calculo Mermelada.xlsx
+++ b/No Code/Calculo Mermelada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilith\Desktop\Proyecto-Quimica-Mermelada\No Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5a230e1bdf9cfeb/Documentos/iteso/visual/WEB/Proyecto-Quimica-Mermelada/No Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D579DC-01AA-41BD-871A-6D9BBA53328B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{99D579DC-01AA-41BD-871A-6D9BBA53328B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F409F2C9-68B0-4007-BC91-1157816EBC86}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6DFA522A-53B6-478F-9D27-66162FDD3BAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -136,9 +136,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="172" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -220,7 +220,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -258,13 +258,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,25 +590,25 @@
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" style="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -661,7 +661,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="3">
-        <v>500</v>
+        <v>436</v>
       </c>
       <c r="J3" s="7">
         <f>C20</f>
@@ -676,10 +676,10 @@
       </c>
       <c r="N3" s="16">
         <f>J4+I4</f>
-        <v>28510</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -703,7 +703,7 @@
       </c>
       <c r="I4" s="16">
         <f>I3*I17</f>
-        <v>25000</v>
+        <v>21800</v>
       </c>
       <c r="J4" s="16">
         <f>I18*J3</f>
@@ -722,7 +722,7 @@
         <v>32500</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -743,10 +743,10 @@
       </c>
       <c r="N5" s="15">
         <f>N4-N3</f>
-        <v>3990</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>7190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -766,7 +766,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -785,7 +785,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>5</v>
       </c>
@@ -823,7 +823,7 @@
         <v>25310</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -867,7 +867,7 @@
         <v>32500</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -894,7 +894,7 @@
         <v>7190</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -914,7 +914,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -933,7 +933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>21</v>
       </c>
@@ -971,7 +971,7 @@
         <v>25310</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>32500</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>9</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>7190</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>10</v>
       </c>
@@ -1065,7 +1065,7 @@
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1076,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>11</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>175.5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>

</xml_diff>